<commit_message>
ongoing work on data inspection
</commit_message>
<xml_diff>
--- a/LCOPT-data-dict.xlsx
+++ b/LCOPT-data-dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/projects/lc2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264FE613-DEED-4449-B998-AAB76B48E45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904B4F79-47B5-E14F-BC59-04E9EEECB9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="260" yWindow="-19960" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LCOPT-data-dict" sheetId="1" r:id="rId1"/>
@@ -3413,10 +3413,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q353"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D220" sqref="D220"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3425,6 +3426,7 @@
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
     <col min="3" max="6" width="12.5" customWidth="1"/>
     <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3449,7 +3451,7 @@
       <c r="G1" t="s">
         <v>837</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I1" t="s">
@@ -3480,7 +3482,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -3500,7 +3502,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -3517,7 +3519,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -3534,7 +3536,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -3551,7 +3553,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -3568,7 +3570,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -3585,7 +3587,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3602,7 +3604,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -3619,7 +3621,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -3636,7 +3638,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -3653,7 +3655,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -3670,7 +3672,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -3687,7 +3689,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -3704,7 +3706,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -3721,7 +3723,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -3738,7 +3740,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -3755,7 +3757,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -3772,7 +3774,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -3789,7 +3791,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -3806,7 +3808,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -3823,7 +3825,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -3840,7 +3842,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -3857,7 +3859,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -3874,7 +3876,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -3891,7 +3893,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -3911,7 +3913,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>65</v>
       </c>
@@ -3928,7 +3930,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -3951,7 +3953,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>70</v>
       </c>
@@ -3974,7 +3976,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>72</v>
       </c>
@@ -4000,7 +4002,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>76</v>
       </c>
@@ -4020,7 +4022,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -4043,7 +4045,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>81</v>
       </c>
@@ -4060,7 +4062,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>83</v>
       </c>
@@ -4083,7 +4085,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -4106,7 +4108,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>87</v>
       </c>
@@ -4132,7 +4134,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>89</v>
       </c>
@@ -4152,7 +4154,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>90</v>
       </c>
@@ -4169,7 +4171,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>93</v>
       </c>
@@ -4195,7 +4197,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>96</v>
       </c>
@@ -4215,7 +4217,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -4247,7 +4249,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>101</v>
       </c>
@@ -4270,7 +4272,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>104</v>
       </c>
@@ -4293,7 +4295,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>107</v>
       </c>
@@ -4316,7 +4318,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>109</v>
       </c>
@@ -4336,7 +4338,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>112</v>
       </c>
@@ -4356,7 +4358,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>114</v>
       </c>
@@ -4379,7 +4381,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>118</v>
       </c>
@@ -4402,7 +4404,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>122</v>
       </c>
@@ -4422,7 +4424,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>124</v>
       </c>
@@ -4442,7 +4444,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>126</v>
       </c>
@@ -4459,7 +4461,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>129</v>
       </c>
@@ -4482,7 +4484,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>132</v>
       </c>
@@ -4524,11 +4526,11 @@
       <c r="G54" t="s">
         <v>136</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H54" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>138</v>
       </c>
@@ -4551,7 +4553,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>140</v>
       </c>
@@ -4574,7 +4576,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>141</v>
       </c>
@@ -4597,7 +4599,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>142</v>
       </c>
@@ -4620,7 +4622,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>143</v>
       </c>
@@ -4643,7 +4645,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>144</v>
       </c>
@@ -4666,7 +4668,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>145</v>
       </c>
@@ -4689,7 +4691,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>146</v>
       </c>
@@ -4712,7 +4714,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>147</v>
       </c>
@@ -4735,7 +4737,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>148</v>
       </c>
@@ -4758,7 +4760,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>149</v>
       </c>
@@ -4781,7 +4783,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>150</v>
       </c>
@@ -4804,7 +4806,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>151</v>
       </c>
@@ -4827,7 +4829,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>152</v>
       </c>
@@ -4850,7 +4852,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>153</v>
       </c>
@@ -4873,7 +4875,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>154</v>
       </c>
@@ -4890,7 +4892,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>157</v>
       </c>
@@ -4919,7 +4921,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>161</v>
       </c>
@@ -4951,7 +4953,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>165</v>
       </c>
@@ -4983,7 +4985,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>167</v>
       </c>
@@ -5015,7 +5017,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>169</v>
       </c>
@@ -5047,7 +5049,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>171</v>
       </c>
@@ -5079,7 +5081,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>173</v>
       </c>
@@ -5111,7 +5113,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>175</v>
       </c>
@@ -5143,7 +5145,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>177</v>
       </c>
@@ -5175,7 +5177,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>179</v>
       </c>
@@ -5207,7 +5209,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="81" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>181</v>
       </c>
@@ -5239,7 +5241,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>183</v>
       </c>
@@ -5271,7 +5273,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>185</v>
       </c>
@@ -5303,7 +5305,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>187</v>
       </c>
@@ -5335,7 +5337,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>189</v>
       </c>
@@ -5367,7 +5369,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>191</v>
       </c>
@@ -5399,7 +5401,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>193</v>
       </c>
@@ -5431,7 +5433,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>195</v>
       </c>
@@ -5463,7 +5465,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>197</v>
       </c>
@@ -5495,7 +5497,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>199</v>
       </c>
@@ -5527,7 +5529,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>201</v>
       </c>
@@ -5559,7 +5561,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="92" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>203</v>
       </c>
@@ -5591,7 +5593,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="93" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>205</v>
       </c>
@@ -5623,7 +5625,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="94" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>207</v>
       </c>
@@ -5655,7 +5657,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="95" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>209</v>
       </c>
@@ -5687,7 +5689,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="96" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>211</v>
       </c>
@@ -5719,7 +5721,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="97" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>213</v>
       </c>
@@ -5751,7 +5753,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="98" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>215</v>
       </c>
@@ -5783,7 +5785,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="99" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>217</v>
       </c>
@@ -5815,7 +5817,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>219</v>
       </c>
@@ -5844,7 +5846,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="101" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>223</v>
       </c>
@@ -5873,7 +5875,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="102" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>225</v>
       </c>
@@ -5902,7 +5904,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="103" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>227</v>
       </c>
@@ -5931,7 +5933,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>229</v>
       </c>
@@ -5960,7 +5962,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="105" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>231</v>
       </c>
@@ -5989,7 +5991,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="106" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>233</v>
       </c>
@@ -6018,7 +6020,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="107" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>235</v>
       </c>
@@ -6063,11 +6065,11 @@
       <c r="G108" t="s">
         <v>136</v>
       </c>
-      <c r="H108" t="s">
+      <c r="H108" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="109" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>239</v>
       </c>
@@ -6096,7 +6098,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="110" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>244</v>
       </c>
@@ -6125,7 +6127,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="111" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>246</v>
       </c>
@@ -6154,7 +6156,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="112" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>248</v>
       </c>
@@ -6183,7 +6185,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>250</v>
       </c>
@@ -6212,7 +6214,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>252</v>
       </c>
@@ -6241,7 +6243,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="115" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>254</v>
       </c>
@@ -6270,7 +6272,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="116" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>256</v>
       </c>
@@ -6296,7 +6298,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="117" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>260</v>
       </c>
@@ -6322,7 +6324,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="118" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>263</v>
       </c>
@@ -6348,7 +6350,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="119" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>266</v>
       </c>
@@ -6374,7 +6376,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="120" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>269</v>
       </c>
@@ -6400,7 +6402,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="121" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>272</v>
       </c>
@@ -6429,7 +6431,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="122" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>276</v>
       </c>
@@ -6458,7 +6460,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="123" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>281</v>
       </c>
@@ -6487,7 +6489,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="124" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>283</v>
       </c>
@@ -6516,7 +6518,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="125" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>285</v>
       </c>
@@ -6545,7 +6547,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="126" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>287</v>
       </c>
@@ -6574,7 +6576,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="127" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>291</v>
       </c>
@@ -6603,7 +6605,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="128" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>293</v>
       </c>
@@ -6632,7 +6634,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="129" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>295</v>
       </c>
@@ -6661,7 +6663,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="130" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>297</v>
       </c>
@@ -6690,7 +6692,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="131" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>300</v>
       </c>
@@ -6719,7 +6721,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="132" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>302</v>
       </c>
@@ -6748,7 +6750,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="133" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>304</v>
       </c>
@@ -6777,7 +6779,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="134" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>306</v>
       </c>
@@ -6806,7 +6808,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="135" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>309</v>
       </c>
@@ -6835,7 +6837,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="136" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>311</v>
       </c>
@@ -6864,7 +6866,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="137" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>313</v>
       </c>
@@ -6893,7 +6895,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="138" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>315</v>
       </c>
@@ -6922,7 +6924,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="139" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>319</v>
       </c>
@@ -6951,7 +6953,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="140" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>323</v>
       </c>
@@ -6980,7 +6982,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="141" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>326</v>
       </c>
@@ -7009,7 +7011,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="142" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>328</v>
       </c>
@@ -7035,7 +7037,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="143" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>332</v>
       </c>
@@ -7061,7 +7063,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="144" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>334</v>
       </c>
@@ -7087,7 +7089,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="145" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>336</v>
       </c>
@@ -7113,7 +7115,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="146" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>338</v>
       </c>
@@ -7142,7 +7144,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="147" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>341</v>
       </c>
@@ -7171,7 +7173,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="148" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>343</v>
       </c>
@@ -7200,7 +7202,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="149" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>345</v>
       </c>
@@ -7229,7 +7231,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="150" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>347</v>
       </c>
@@ -7258,7 +7260,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="151" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>351</v>
       </c>
@@ -7284,7 +7286,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="152" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>355</v>
       </c>
@@ -7310,7 +7312,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="153" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>357</v>
       </c>
@@ -7336,7 +7338,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="154" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>359</v>
       </c>
@@ -7362,7 +7364,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="155" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>361</v>
       </c>
@@ -7388,7 +7390,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="156" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>363</v>
       </c>
@@ -7414,7 +7416,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="157" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>365</v>
       </c>
@@ -7440,7 +7442,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="158" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>367</v>
       </c>
@@ -7466,7 +7468,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="159" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>369</v>
       </c>
@@ -7492,7 +7494,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="160" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>371</v>
       </c>
@@ -7509,7 +7511,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="161" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>373</v>
       </c>
@@ -7535,7 +7537,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="162" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>376</v>
       </c>
@@ -7552,7 +7554,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="163" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>379</v>
       </c>
@@ -7581,7 +7583,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="164" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>381</v>
       </c>
@@ -7610,7 +7612,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="165" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>384</v>
       </c>
@@ -7642,7 +7644,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="166" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>387</v>
       </c>
@@ -7674,7 +7676,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="167" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>390</v>
       </c>
@@ -7703,7 +7705,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="168" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>393</v>
       </c>
@@ -7735,7 +7737,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="169" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>395</v>
       </c>
@@ -7764,7 +7766,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="170" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>397</v>
       </c>
@@ -7796,7 +7798,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="171" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>399</v>
       </c>
@@ -7825,7 +7827,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="172" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>401</v>
       </c>
@@ -7857,7 +7859,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="173" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>403</v>
       </c>
@@ -7886,7 +7888,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="174" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>405</v>
       </c>
@@ -7918,7 +7920,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="175" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>407</v>
       </c>
@@ -7947,7 +7949,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="176" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>409</v>
       </c>
@@ -7979,7 +7981,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="177" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>412</v>
       </c>
@@ -8011,7 +8013,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="178" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>415</v>
       </c>
@@ -8043,7 +8045,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="179" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>418</v>
       </c>
@@ -8075,7 +8077,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="180" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>421</v>
       </c>
@@ -8107,7 +8109,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="181" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>424</v>
       </c>
@@ -8139,7 +8141,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="182" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>426</v>
       </c>
@@ -8171,7 +8173,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="183" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>428</v>
       </c>
@@ -8203,7 +8205,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="184" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>430</v>
       </c>
@@ -8235,7 +8237,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="185" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>433</v>
       </c>
@@ -8267,7 +8269,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="186" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>436</v>
       </c>
@@ -8299,7 +8301,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="187" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>438</v>
       </c>
@@ -8331,7 +8333,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="188" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>441</v>
       </c>
@@ -8363,7 +8365,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="189" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>443</v>
       </c>
@@ -8395,7 +8397,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="190" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>445</v>
       </c>
@@ -8427,7 +8429,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="191" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>448</v>
       </c>
@@ -8459,7 +8461,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="192" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>450</v>
       </c>
@@ -8491,7 +8493,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="193" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>452</v>
       </c>
@@ -8523,7 +8525,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="194" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>454</v>
       </c>
@@ -8555,7 +8557,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="195" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>456</v>
       </c>
@@ -8587,7 +8589,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="196" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>459</v>
       </c>
@@ -8616,7 +8618,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="197" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>461</v>
       </c>
@@ -8648,7 +8650,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="198" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>463</v>
       </c>
@@ -8680,7 +8682,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="199" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>466</v>
       </c>
@@ -8712,7 +8714,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="200" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>468</v>
       </c>
@@ -8744,7 +8746,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="201" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>470</v>
       </c>
@@ -8776,7 +8778,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="202" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>472</v>
       </c>
@@ -8808,7 +8810,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="203" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>475</v>
       </c>
@@ -8840,7 +8842,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="204" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>479</v>
       </c>
@@ -8872,7 +8874,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="205" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>482</v>
       </c>
@@ -8904,7 +8906,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="206" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>484</v>
       </c>
@@ -8927,7 +8929,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="207" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>486</v>
       </c>
@@ -8950,7 +8952,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="208" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>488</v>
       </c>
@@ -8973,7 +8975,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="209" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>490</v>
       </c>
@@ -8996,7 +8998,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="210" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>492</v>
       </c>
@@ -9019,7 +9021,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="211" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>494</v>
       </c>
@@ -9042,7 +9044,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="212" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>496</v>
       </c>
@@ -9065,7 +9067,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="213" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>498</v>
       </c>
@@ -9088,7 +9090,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="214" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>500</v>
       </c>
@@ -9127,11 +9129,11 @@
       <c r="G215" t="s">
         <v>136</v>
       </c>
-      <c r="H215" t="s">
+      <c r="H215" s="1" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="216" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>504</v>
       </c>
@@ -9154,7 +9156,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="217" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>506</v>
       </c>
@@ -9177,7 +9179,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="218" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>508</v>
       </c>
@@ -9200,7 +9202,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="219" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>510</v>
       </c>
@@ -9223,7 +9225,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="220" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>512</v>
       </c>
@@ -9240,7 +9242,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="221" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>515</v>
       </c>
@@ -9257,7 +9259,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="222" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>517</v>
       </c>
@@ -9274,7 +9276,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="223" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>519</v>
       </c>
@@ -9297,7 +9299,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="224" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>521</v>
       </c>
@@ -9314,7 +9316,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="225" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>523</v>
       </c>
@@ -9343,7 +9345,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="226" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>524</v>
       </c>
@@ -9372,7 +9374,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="227" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>525</v>
       </c>
@@ -9401,7 +9403,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="228" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>526</v>
       </c>
@@ -9430,7 +9432,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="229" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>527</v>
       </c>
@@ -9459,7 +9461,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="230" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>528</v>
       </c>
@@ -9488,7 +9490,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="231" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>529</v>
       </c>
@@ -9517,7 +9519,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="232" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>530</v>
       </c>
@@ -9546,7 +9548,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="233" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>531</v>
       </c>
@@ -9585,11 +9587,11 @@
       <c r="G234" t="s">
         <v>136</v>
       </c>
-      <c r="H234" t="s">
+      <c r="H234" s="1" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="235" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>535</v>
       </c>
@@ -9612,7 +9614,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="236" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>537</v>
       </c>
@@ -9641,7 +9643,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="237" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>541</v>
       </c>
@@ -9670,7 +9672,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="238" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>543</v>
       </c>
@@ -9699,7 +9701,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="239" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>545</v>
       </c>
@@ -9728,7 +9730,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="240" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>547</v>
       </c>
@@ -9757,7 +9759,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="241" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>549</v>
       </c>
@@ -9786,7 +9788,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="242" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>551</v>
       </c>
@@ -9815,7 +9817,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="243" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>553</v>
       </c>
@@ -9844,7 +9846,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="244" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>555</v>
       </c>
@@ -9873,7 +9875,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="245" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>557</v>
       </c>
@@ -9902,7 +9904,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="246" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>559</v>
       </c>
@@ -9931,7 +9933,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="247" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>561</v>
       </c>
@@ -9960,7 +9962,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="248" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>563</v>
       </c>
@@ -9989,7 +9991,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="249" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>565</v>
       </c>
@@ -10018,7 +10020,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="250" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>567</v>
       </c>
@@ -10047,7 +10049,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="251" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>569</v>
       </c>
@@ -10076,7 +10078,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="252" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>571</v>
       </c>
@@ -10105,7 +10107,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="253" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>573</v>
       </c>
@@ -10134,7 +10136,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="254" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>575</v>
       </c>
@@ -10163,7 +10165,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="255" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>577</v>
       </c>
@@ -10192,7 +10194,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="256" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>579</v>
       </c>
@@ -10221,7 +10223,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="257" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>581</v>
       </c>
@@ -10250,7 +10252,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="258" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>583</v>
       </c>
@@ -10279,7 +10281,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="259" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>585</v>
       </c>
@@ -10308,7 +10310,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="260" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>587</v>
       </c>
@@ -10337,7 +10339,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="261" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>589</v>
       </c>
@@ -10366,7 +10368,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="262" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>591</v>
       </c>
@@ -10395,7 +10397,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="263" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>593</v>
       </c>
@@ -10424,7 +10426,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="264" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>595</v>
       </c>
@@ -10453,7 +10455,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="265" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>597</v>
       </c>
@@ -10482,7 +10484,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="266" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>599</v>
       </c>
@@ -10511,7 +10513,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="267" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>601</v>
       </c>
@@ -10540,7 +10542,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="268" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>603</v>
       </c>
@@ -10569,7 +10571,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="269" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>605</v>
       </c>
@@ -10598,7 +10600,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="270" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>607</v>
       </c>
@@ -10627,7 +10629,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="271" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>609</v>
       </c>
@@ -10656,7 +10658,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="272" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>611</v>
       </c>
@@ -10685,7 +10687,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="273" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>613</v>
       </c>
@@ -10714,7 +10716,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="274" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>290</v>
       </c>
@@ -10743,7 +10745,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="275" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>616</v>
       </c>
@@ -10772,7 +10774,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="276" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>618</v>
       </c>
@@ -10801,7 +10803,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="277" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>620</v>
       </c>
@@ -10830,7 +10832,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="278" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>622</v>
       </c>
@@ -10859,7 +10861,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="279" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>624</v>
       </c>
@@ -10888,7 +10890,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="280" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>626</v>
       </c>
@@ -10917,7 +10919,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="281" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>628</v>
       </c>
@@ -10946,7 +10948,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="282" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>630</v>
       </c>
@@ -10975,7 +10977,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="283" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>632</v>
       </c>
@@ -11004,7 +11006,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="284" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>634</v>
       </c>
@@ -11033,7 +11035,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="285" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>636</v>
       </c>
@@ -11062,7 +11064,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="286" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>638</v>
       </c>
@@ -11091,7 +11093,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="287" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>640</v>
       </c>
@@ -11120,7 +11122,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="288" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:16" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>642</v>
       </c>
@@ -11143,7 +11145,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="289" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>644</v>
       </c>
@@ -11169,7 +11171,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="290" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>647</v>
       </c>
@@ -11198,7 +11200,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="291" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>649</v>
       </c>
@@ -11224,7 +11226,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="292" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>652</v>
       </c>
@@ -11250,7 +11252,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="293" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>655</v>
       </c>
@@ -11279,7 +11281,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="294" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>658</v>
       </c>
@@ -11299,7 +11301,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="295" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>660</v>
       </c>
@@ -11328,7 +11330,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="296" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>662</v>
       </c>
@@ -11354,7 +11356,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="297" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>665</v>
       </c>
@@ -11374,7 +11376,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="298" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>667</v>
       </c>
@@ -11406,7 +11408,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="299" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>670</v>
       </c>
@@ -11438,7 +11440,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="300" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>672</v>
       </c>
@@ -11467,7 +11469,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="301" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>674</v>
       </c>
@@ -11499,7 +11501,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="302" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>676</v>
       </c>
@@ -11531,7 +11533,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="303" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>679</v>
       </c>
@@ -11563,7 +11565,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="304" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>682</v>
       </c>
@@ -11595,7 +11597,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="305" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>684</v>
       </c>
@@ -11618,7 +11620,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="306" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>687</v>
       </c>
@@ -11641,7 +11643,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="307" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>690</v>
       </c>
@@ -11664,7 +11666,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="308" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>693</v>
       </c>
@@ -11693,7 +11695,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="309" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>695</v>
       </c>
@@ -11719,7 +11721,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="310" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>698</v>
       </c>
@@ -11745,7 +11747,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="311" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>701</v>
       </c>
@@ -11774,7 +11776,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="312" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>703</v>
       </c>
@@ -11800,7 +11802,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="313" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>704</v>
       </c>
@@ -11826,7 +11828,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="314" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>705</v>
       </c>
@@ -11855,7 +11857,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="315" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>707</v>
       </c>
@@ -11881,7 +11883,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="316" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>708</v>
       </c>
@@ -11907,7 +11909,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="317" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>709</v>
       </c>
@@ -11936,7 +11938,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="318" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>711</v>
       </c>
@@ -11962,7 +11964,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="319" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>712</v>
       </c>
@@ -11988,7 +11990,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="320" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>713</v>
       </c>
@@ -12017,7 +12019,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="321" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>715</v>
       </c>
@@ -12043,7 +12045,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="322" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>716</v>
       </c>
@@ -12069,7 +12071,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="323" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>717</v>
       </c>
@@ -12095,7 +12097,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="324" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>720</v>
       </c>
@@ -12118,7 +12120,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="325" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>722</v>
       </c>
@@ -12147,7 +12149,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="326" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>724</v>
       </c>
@@ -12176,7 +12178,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="327" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>726</v>
       </c>
@@ -12199,7 +12201,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="328" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>728</v>
       </c>
@@ -12222,7 +12224,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="329" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>731</v>
       </c>
@@ -12261,11 +12263,11 @@
       <c r="G330" t="s">
         <v>136</v>
       </c>
-      <c r="H330" t="s">
+      <c r="H330" s="1" t="s">
         <v>735</v>
       </c>
     </row>
-    <row r="331" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>736</v>
       </c>
@@ -12288,7 +12290,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="332" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>739</v>
       </c>
@@ -12320,7 +12322,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="333" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>742</v>
       </c>
@@ -12343,7 +12345,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="334" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>745</v>
       </c>
@@ -12375,7 +12377,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="335" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>748</v>
       </c>
@@ -12398,7 +12400,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="336" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:13" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>751</v>
       </c>
@@ -12430,7 +12432,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="337" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:14" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>754</v>
       </c>
@@ -12462,7 +12464,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="338" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:14" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>756</v>
       </c>
@@ -12494,7 +12496,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="339" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:14" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>758</v>
       </c>
@@ -12526,7 +12528,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="340" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:14" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>761</v>
       </c>
@@ -12574,11 +12576,11 @@
       <c r="G341" t="s">
         <v>136</v>
       </c>
-      <c r="H341" t="s">
+      <c r="H341" s="1" t="s">
         <v>765</v>
       </c>
     </row>
-    <row r="342" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:14" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>766</v>
       </c>
@@ -12598,7 +12600,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="343" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:14" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>768</v>
       </c>
@@ -12624,7 +12626,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="344" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:14" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>773</v>
       </c>
@@ -12650,7 +12652,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="345" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:14" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>776</v>
       </c>
@@ -12676,7 +12678,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="346" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:14" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>779</v>
       </c>
@@ -12699,7 +12701,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="347" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:14" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>782</v>
       </c>
@@ -12725,7 +12727,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="348" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:14" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>785</v>
       </c>
@@ -12742,7 +12744,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="349" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:14" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>787</v>
       </c>
@@ -12759,7 +12761,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="350" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:14" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>789</v>
       </c>
@@ -12785,7 +12787,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="351" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:14" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>791</v>
       </c>
@@ -12805,7 +12807,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="352" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:14" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>793</v>
       </c>
@@ -12825,7 +12827,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="353" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:8" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>796</v>
       </c>
@@ -12843,7 +12845,18 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q353" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:Q353" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="6">
+      <filters>
+        <filter val="notes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>